<commit_message>
Changes have been made to the Implementation plan
</commit_message>
<xml_diff>
--- a/Implementation Plan.xlsx
+++ b/Implementation Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\samuelparkin1\ccc_coursework\python\T1A3 - Terminal Application\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D9AC1A-5ED0-4702-BB4F-A0E9617B86DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8005345A-3C59-4EB0-9DBD-11EE5524EE54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{159876CB-0B65-44F8-9DE3-DF5C20F5338D}"/>
   </bookViews>
@@ -69,9 +69,6 @@
     <t xml:space="preserve">Medium </t>
   </si>
   <si>
-    <t>A start game prompt</t>
-  </si>
-  <si>
     <t xml:space="preserve">High </t>
   </si>
   <si>
@@ -166,6 +163,9 @@
   </si>
   <si>
     <t xml:space="preserve">To be done after main game and list feature. If unable to get this completed due to deadline app can still partially work. </t>
+  </si>
+  <si>
+    <t>A start game feature</t>
   </si>
 </sst>
 </file>
@@ -538,7 +538,7 @@
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,7 +569,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -581,7 +581,7 @@
         <v>44392</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -605,81 +605,81 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" s="3">
         <v>44392</v>
       </c>
       <c r="E7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D13" s="3">
         <v>44389</v>
       </c>
       <c r="E13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -687,49 +687,49 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D20" s="3">
         <v>44391</v>
       </c>
       <c r="E20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -737,21 +737,21 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" t="s">
         <v>33</v>
-      </c>
-      <c r="B28" t="s">
-        <v>34</v>
       </c>
       <c r="D28" s="3">
         <v>44393</v>
       </c>
       <c r="E28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B29" t="s">
         <v>10</v>
@@ -767,19 +767,19 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
       </c>
       <c r="C31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D31" s="3">
         <v>44393</v>
       </c>
       <c r="E31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
files have been moved into Documentation folder
</commit_message>
<xml_diff>
--- a/Implementation Plan.xlsx
+++ b/Implementation Plan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\samuelparkin1\ccc_coursework\python\T1A3 - Terminal Application\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\samuelparkin1\ccc_coursework\python\T1A3-Terminal_Application\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8005345A-3C59-4EB0-9DBD-11EE5524EE54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CF38C99-CA42-4A59-8BEB-B0CB7C8C026F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{159876CB-0B65-44F8-9DE3-DF5C20F5338D}"/>
+    <workbookView xWindow="31185" yWindow="285" windowWidth="21600" windowHeight="11505" xr2:uid="{159876CB-0B65-44F8-9DE3-DF5C20F5338D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="44">
   <si>
     <t>Implementation of different features</t>
   </si>
@@ -90,42 +90,24 @@
     <t>-needs to make sure numbers aren’t entered</t>
   </si>
   <si>
-    <t xml:space="preserve">- Create a temporary list of all previous and new the player names. </t>
-  </si>
-  <si>
     <t>- Creates a list of descritive words used within each facial features dictionay</t>
   </si>
   <si>
-    <t xml:space="preserve">- Need to ensure that the  descritive words aren't repeated within their lists </t>
-  </si>
-  <si>
     <t xml:space="preserve">This will be needed to be completed prior to starting the the main game feature. </t>
   </si>
   <si>
     <t xml:space="preserve">Main game feature </t>
   </si>
   <si>
-    <t>-Communicate to the user the rules of the game</t>
-  </si>
-  <si>
     <t>10 hours</t>
   </si>
   <si>
-    <t xml:space="preserve">- It will need to be able to generate questions with a randon feature  </t>
-  </si>
-  <si>
     <t xml:space="preserve">Bash script </t>
   </si>
   <si>
     <t xml:space="preserve">2 hours </t>
   </si>
   <si>
-    <t xml:space="preserve">- it will need to take in user responses and ensure no errors accour </t>
-  </si>
-  <si>
-    <t>- needs remove the feature it has asked in order not to ask it again</t>
-  </si>
-  <si>
     <t xml:space="preserve">- Has a counter to figure out how many questions have been asked. </t>
   </si>
   <si>
@@ -156,16 +138,34 @@
     <t xml:space="preserve">6 hours </t>
   </si>
   <si>
-    <t>-Create a list for names of all the player and fictional character.</t>
-  </si>
-  <si>
-    <t>List feature</t>
-  </si>
-  <si>
     <t xml:space="preserve">To be done after main game and list feature. If unable to get this completed due to deadline app can still partially work. </t>
   </si>
   <si>
     <t>A start game feature</t>
+  </si>
+  <si>
+    <t>- A default list of 30 names and facial features need to generated</t>
+  </si>
+  <si>
+    <t>List and dictionies data base.</t>
+  </si>
+  <si>
+    <t>- Create a list for names of all the player and fictional character.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Need to ensure that the descritive words aren't repeated within their lists </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-Communicate to the user the how the game works. </t>
+  </si>
+  <si>
+    <t>- It will need to be able to generate randon questions</t>
+  </si>
+  <si>
+    <t>- it will need to take in user responses and ensure no errors occor</t>
+  </si>
+  <si>
+    <t>- needs remove the question it has asked in order not to ask it again</t>
   </si>
 </sst>
 </file>
@@ -535,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7B731F4-D78D-4051-8B51-0EB0BFE561BF}">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,7 +569,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -617,7 +617,7 @@
         <v>44392</v>
       </c>
       <c r="E7" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -637,29 +637,29 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D13" s="3">
         <v>44389</v>
       </c>
       <c r="E13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -669,117 +669,117 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="3">
+        <v>44391</v>
+      </c>
+      <c r="E19" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" t="s">
-        <v>24</v>
-      </c>
-      <c r="D20" s="3">
-        <v>44391</v>
-      </c>
-      <c r="E20" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>30</v>
-      </c>
+      <c r="A26" s="2"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
+      <c r="A27" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" s="3">
+        <v>44393</v>
+      </c>
+      <c r="E27" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B28" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="D28" s="3">
         <v>44393</v>
       </c>
-      <c r="E28" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B29" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="3">
-        <v>44393</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
+      </c>
+      <c r="B30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" s="3">
+        <v>44393</v>
+      </c>
+      <c r="E30" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B31" t="s">
-        <v>10</v>
-      </c>
-      <c r="C31" t="s">
-        <v>27</v>
-      </c>
-      <c r="D31" s="3">
-        <v>44393</v>
-      </c>
-      <c r="E31" t="s">
-        <v>36</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -839,11 +839,6 @@
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>